<commit_message>
fix(publipostage): Refactor synthetic array
</commit_message>
<xml_diff>
--- a/publipostage2/003vg9w96/liste_essais_cliniques_identifies_003vg9w96.xlsx
+++ b/publipostage2/003vg9w96/liste_essais_cliniques_identifies_003vg9w96.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,50 +446,55 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>statut_name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>NCTId</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>eudraCT</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>CTIS</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>completion_year</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>clinical_trial_title</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>acronym</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>results_1y</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>results_3y</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>results</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>intervention_type</t>
         </is>
@@ -508,36 +513,41 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>pas de résultat ni de publication</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>NCT00439582</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
         <is>
           <t>2005</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Comparative Effect of 2 Different Sources of Trans Fatty Acid (Milk Fat vs Hydrogenated Oil)on Cardiovascular Risk Factors in Healthy Humans</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>TRANSFACT1</t>
         </is>
       </c>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
       <c r="J2" t="b">
         <v>0</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" t="b">
+        <v>0</v>
+      </c>
+      <c r="M2" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -556,32 +566,37 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>NCT00873951</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
         <is>
           <t>2008</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Influence of Protein Hydrolysis on Dietary Protein Digestibility and Metabolism in Healthy Subjects</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="b">
         <v>0</v>
       </c>
       <c r="K3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L3" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -600,36 +615,41 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>pas de résultat ni de publication</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>NCT00685581</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
         <is>
           <t>2008</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Rationale, Study Design and Baseline Data of the TRANSQUAL Clinical Trial: A Study to Evaluate the Impact of Different Milk Fatty Acid Profiles on Cardiovascular Risk Factors in Healthy Volunteers; Focus on Trans Fatty Acids</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>TRANSQUAL WPC</t>
         </is>
       </c>
-      <c r="I4" t="b">
-        <v>0</v>
-      </c>
       <c r="J4" t="b">
         <v>0</v>
       </c>
       <c r="K4" t="b">
         <v>0</v>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -648,32 +668,37 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>NCT00617435</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
         <is>
           <t>2009</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr">
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
         <is>
           <t>Trans-Insulin</t>
         </is>
       </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
       <c r="J5" t="b">
         <v>0</v>
       </c>
       <c r="K5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -692,28 +717,33 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>NCT00931151</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr">
         <is>
           <t>2009</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="b">
         <v>0</v>
       </c>
       <c r="K6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="L6" t="b">
+        <v>1</v>
+      </c>
+      <c r="M6" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -732,28 +762,33 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté dans les 36 mois</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>NCT00862329</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
         <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="b">
-        <v>0</v>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="b">
         <v>1</v>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L7" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -772,36 +807,41 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>pas de résultat ni de publication</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>NCT00690781</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
         <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Effect of Milk Proteins and Protein Feeding Pattern on Body Composition and Protein Metabolism in Energy Restricted Obese Subjects</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>SURPROL-CF-H</t>
         </is>
       </c>
-      <c r="I8" t="b">
-        <v>0</v>
-      </c>
       <c r="J8" t="b">
         <v>0</v>
       </c>
       <c r="K8" t="b">
         <v>0</v>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -820,36 +860,41 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>pas de résultat ni de publication</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>NCT01209572</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
         <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Modelling of 24h Energy Expenditure From Heart Rate, Actimetry and Other Parameters Recorded Under Free-living Conditions</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Modelheart</t>
         </is>
       </c>
-      <c r="I9" t="b">
-        <v>0</v>
-      </c>
       <c r="J9" t="b">
         <v>0</v>
       </c>
       <c r="K9" t="b">
         <v>0</v>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9" t="inlineStr">
         <is>
           <t>DEVICE</t>
         </is>
@@ -868,36 +913,41 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>NCT00994526</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr">
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
         <is>
           <t>2010</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>Effect of Processed Meat on Colorectal Carcinogenesis. Study of Mechanisms. Choice of Preventive Strategies</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Hemcancer</t>
         </is>
       </c>
-      <c r="I10" t="b">
-        <v>0</v>
-      </c>
       <c r="J10" t="b">
         <v>0</v>
       </c>
       <c r="K10" t="b">
-        <v>1</v>
-      </c>
-      <c r="L10" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="L10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
@@ -916,32 +966,37 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>pas de résultat ni de publication</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>NCT01995162</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
         <is>
           <t>2013</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>A Smartphone Application to Evaluate Energy Expenditure and Duration of Moderate-intensity Activities in Free-living Conditions (eMouve 2)</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="b">
-        <v>0</v>
-      </c>
+      <c r="I11" t="inlineStr"/>
       <c r="J11" t="b">
         <v>0</v>
       </c>
       <c r="K11" t="b">
         <v>0</v>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="L11" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" t="inlineStr">
         <is>
           <t>DEVICE</t>
         </is>
@@ -960,32 +1015,37 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>pas de résultat ni de publication</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>NCT01995253</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
         <is>
           <t>2013</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>A Smartphone Application to Evaluate Energy Expenditure and Duration of Moderate-intensity Activities</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="b">
-        <v>0</v>
-      </c>
+      <c r="I12" t="inlineStr"/>
       <c r="J12" t="b">
         <v>0</v>
       </c>
       <c r="K12" t="b">
         <v>0</v>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+      <c r="M12" t="inlineStr">
         <is>
           <t>DEVICE</t>
         </is>
@@ -1004,32 +1064,37 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>pas de résultat ni de publication</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>NCT02473302</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>Preventive Strategies in Colorectal Carcinogenesis Production and Meat Processing</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="b">
-        <v>0</v>
-      </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="b">
         <v>0</v>
       </c>
       <c r="K13" t="b">
         <v>0</v>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+      <c r="M13" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
@@ -1048,32 +1113,37 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté dans les 36 mois</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>NCT02354794</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr">
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>Effect of Oral Supplementation With One Form of L-arginine on Vascular Endothelial Function in Healthy Subjects Featuring Risk Factors Related to the Metabolic Syndrome.</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="b">
-        <v>0</v>
-      </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K14" t="b">
         <v>1</v>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="L14" t="b">
+        <v>1</v>
+      </c>
+      <c r="M14" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -1092,32 +1162,37 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>NCT02157805</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>Effect of Technological Processes on Nutritional Quality of Meat Proteins</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="b">
-        <v>0</v>
-      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="b">
         <v>0</v>
       </c>
       <c r="K15" t="b">
-        <v>1</v>
-      </c>
-      <c r="L15" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="L15" t="b">
+        <v>1</v>
+      </c>
+      <c r="M15" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
@@ -1136,36 +1211,41 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>pas de résultat ni de publication</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>NCT02348554</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
         <is>
           <t>2014</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>A Smartphone Application to Evaluate Energy Expenditure and Duration of Activities in Free-living Conditions for Overweight and Obese People (eMouve3)</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>eMouve3</t>
         </is>
       </c>
-      <c r="I16" t="b">
-        <v>0</v>
-      </c>
       <c r="J16" t="b">
         <v>0</v>
       </c>
       <c r="K16" t="b">
         <v>0</v>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="L16" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16" t="inlineStr">
         <is>
           <t>BEHAVIORAL</t>
         </is>
@@ -1184,36 +1264,41 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté dans les 36 mois</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>NCT03492593</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
         <is>
           <t>2016</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>Métabolismes Des caroténoïdes Dans la lumière du Tube Digestif de l'Homme Sain</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>CarotenoiDig</t>
         </is>
       </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
       <c r="J17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="b">
         <v>1</v>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="L17" t="b">
+        <v>1</v>
+      </c>
+      <c r="M17" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
@@ -1232,36 +1317,41 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>NCT03265392</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
         <is>
           <t>2018</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>Digestion: Building a Better Health and Better Understanding the Digestive Processes Thanks to Magnetic Resonance Imaging</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>DECOUVRIR-M</t>
         </is>
       </c>
-      <c r="I18" t="b">
-        <v>0</v>
-      </c>
       <c r="J18" t="b">
         <v>0</v>
       </c>
       <c r="K18" t="b">
-        <v>1</v>
-      </c>
-      <c r="L18" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="L18" t="b">
+        <v>1</v>
+      </c>
+      <c r="M18" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
@@ -1280,32 +1370,37 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté dans les 36 mois</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>NCT03279211</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
         <is>
           <t>2019</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>True Ileal Amino Acid Digestibility of Whey and Zein Proteins in Healthy Volunteers With Naso-ileal Tubes</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
+      <c r="I19" t="inlineStr"/>
       <c r="J19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" t="b">
         <v>1</v>
       </c>
-      <c r="L19" t="inlineStr">
+      <c r="L19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M19" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
@@ -1324,36 +1419,41 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté dans les 36 mois</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>NCT04072770</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr">
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
         <is>
           <t>2020</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>Bioavailability of Protein and Amino Acids of Pea Protein Isolate in Healthy Volunteers</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>Qualipois</t>
         </is>
       </c>
-      <c r="I20" t="b">
-        <v>0</v>
-      </c>
       <c r="J20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K20" t="b">
         <v>1</v>
       </c>
-      <c r="L20" t="inlineStr">
+      <c r="L20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -1372,36 +1472,41 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>pas de résultat ni de publication</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>NCT06624033</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr">
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
         <is>
           <t>2023</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>Single-blind, Randomized, Cross-over Comparative Bioavailability Study About the Kinetics of Plasma Amino Acid Concentrations Subsequent to the Consumption of Innovative Legume-based Products.</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>LEG'UP</t>
         </is>
       </c>
-      <c r="I21" t="b">
-        <v>0</v>
-      </c>
       <c r="J21" t="b">
         <v>0</v>
       </c>
       <c r="K21" t="b">
         <v>0</v>
       </c>
-      <c r="L21" t="inlineStr">
+      <c r="L21" t="b">
+        <v>0</v>
+      </c>
+      <c r="M21" t="inlineStr">
         <is>
           <t>OTHER</t>
         </is>
@@ -1420,36 +1525,41 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>pas de résultat ni de publication</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>NCT05047757</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr">
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
         <is>
           <t>2023</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>Fava Bean Protein and Amino Acid Bioavailability in Healthy Volunteers</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t>Leg4Life</t>
         </is>
       </c>
-      <c r="I22" t="b">
-        <v>0</v>
-      </c>
       <c r="J22" t="b">
         <v>0</v>
       </c>
       <c r="K22" t="b">
         <v>0</v>
       </c>
-      <c r="L22" t="inlineStr">
+      <c r="L22" t="b">
+        <v>0</v>
+      </c>
+      <c r="M22" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -1468,24 +1578,29 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>pas de résultat ni de publication</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>NCT01154608</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
-      <c r="I23" t="b">
-        <v>0</v>
-      </c>
+      <c r="I23" t="inlineStr"/>
       <c r="J23" t="b">
         <v>0</v>
       </c>
       <c r="K23" t="b">
         <v>0</v>
       </c>
-      <c r="L23" t="inlineStr">
+      <c r="L23" t="b">
+        <v>0</v>
+      </c>
+      <c r="M23" t="inlineStr">
         <is>
           <t>DRUG</t>
         </is>
@@ -1504,28 +1619,33 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>NCT02352740</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr">
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
         <is>
           <t>Characterization of the Metabolic Fate of an Oral L-arginine Form in Healthy Subjects Featuring Risk Factors Related to the Metabolic Syndrome.</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="b">
-        <v>0</v>
-      </c>
+      <c r="I24" t="inlineStr"/>
       <c r="J24" t="b">
         <v>0</v>
       </c>
       <c r="K24" t="b">
-        <v>1</v>
-      </c>
-      <c r="L24" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="L24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -1544,28 +1664,33 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>NCT00862017</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr">
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr">
         <is>
           <t>Effect of Monosodium Glutamate on Gastric Emptying and Postprandial Nitrogen in Healthy Volunteers</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="b">
-        <v>0</v>
-      </c>
+      <c r="I25" t="inlineStr"/>
       <c r="J25" t="b">
         <v>0</v>
       </c>
       <c r="K25" t="b">
-        <v>1</v>
-      </c>
-      <c r="L25" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="L25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M25" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>
@@ -1584,24 +1709,29 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>résultat et / ou publication posté</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>NCT01154582</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="b">
-        <v>0</v>
-      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="b">
         <v>0</v>
       </c>
       <c r="K26" t="b">
-        <v>1</v>
-      </c>
-      <c r="L26" t="inlineStr">
+        <v>0</v>
+      </c>
+      <c r="L26" t="b">
+        <v>1</v>
+      </c>
+      <c r="M26" t="inlineStr">
         <is>
           <t>DIETARY_SUPPLEMENT</t>
         </is>

</xml_diff>

<commit_message>
fix(publipostage): Add space before ":"
</commit_message>
<xml_diff>
--- a/publipostage2/003vg9w96/liste_essais_cliniques_identifies_003vg9w96.xlsx
+++ b/publipostage2/003vg9w96/liste_essais_cliniques_identifies_003vg9w96.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="87">
   <si>
     <t>statut</t>
   </si>
@@ -52,13 +52,13 @@
     <t>2</t>
   </si>
   <si>
-    <t>4: pas de résultats postés ni publiés</t>
-  </si>
-  <si>
-    <t>3: résultats postés ou publiés après les 36 mois</t>
-  </si>
-  <si>
-    <t>2: résultats postés ou publiés entre 12 et 36 mois</t>
+    <t>4 : pas de résultats postés ni publiés</t>
+  </si>
+  <si>
+    <t>3 : résultats postés ou publiés après les 36 mois</t>
+  </si>
+  <si>
+    <t>2 : résultats postés ou publiés entre 12 et 36 mois</t>
   </si>
   <si>
     <t>NCT00439582</t>
@@ -76,22 +76,28 @@
     <t>NCT00931151</t>
   </si>
   <si>
+    <t>NCT00690781</t>
+  </si>
+  <si>
     <t>NCT01209572</t>
   </si>
   <si>
+    <t>NCT00994526</t>
+  </si>
+  <si>
     <t>NCT00862329</t>
   </si>
   <si>
-    <t>NCT00690781</t>
-  </si>
-  <si>
-    <t>NCT00994526</t>
+    <t>NCT01995162</t>
   </si>
   <si>
     <t>NCT01995253</t>
   </si>
   <si>
-    <t>NCT01995162</t>
+    <t>NCT02348554</t>
+  </si>
+  <si>
+    <t>NCT02354794</t>
   </si>
   <si>
     <t>NCT02157805</t>
@@ -100,12 +106,6 @@
     <t>NCT02473302</t>
   </si>
   <si>
-    <t>NCT02354794</t>
-  </si>
-  <si>
-    <t>NCT02348554</t>
-  </si>
-  <si>
     <t>NCT03492593</t>
   </si>
   <si>
@@ -124,18 +124,18 @@
     <t>NCT05047757</t>
   </si>
   <si>
+    <t>NCT00862017</t>
+  </si>
+  <si>
     <t>NCT01154608</t>
   </si>
   <si>
+    <t>NCT01154582</t>
+  </si>
+  <si>
     <t>NCT02352740</t>
   </si>
   <si>
-    <t>NCT00862017</t>
-  </si>
-  <si>
-    <t>NCT01154582</t>
-  </si>
-  <si>
     <t>2005</t>
   </si>
   <si>
@@ -178,19 +178,25 @@
     <t>Rationale, Study Design and Baseline Data of the TRANSQUAL Clinical Trial: A Study to Evaluate the Impact of Different Milk Fatty Acid Profiles on Cardiovascular Risk Factors in Healthy Volunteers; Focus on Trans Fatty Acids</t>
   </si>
   <si>
+    <t>Effect of Milk Proteins and Protein Feeding Pattern on Body Composition and Protein Metabolism in Energy Restricted Obese Subjects</t>
+  </si>
+  <si>
     <t>Modelling of 24h Energy Expenditure From Heart Rate, Actimetry and Other Parameters Recorded Under Free-living Conditions</t>
   </si>
   <si>
-    <t>Effect of Milk Proteins and Protein Feeding Pattern on Body Composition and Protein Metabolism in Energy Restricted Obese Subjects</t>
-  </si>
-  <si>
     <t>Effect of Processed Meat on Colorectal Carcinogenesis. Study of Mechanisms. Choice of Preventive Strategies</t>
   </si>
   <si>
+    <t>A Smartphone Application to Evaluate Energy Expenditure and Duration of Moderate-intensity Activities in Free-living Conditions (eMouve 2)</t>
+  </si>
+  <si>
     <t>A Smartphone Application to Evaluate Energy Expenditure and Duration of Moderate-intensity Activities</t>
   </si>
   <si>
-    <t>A Smartphone Application to Evaluate Energy Expenditure and Duration of Moderate-intensity Activities in Free-living Conditions (eMouve 2)</t>
+    <t>A Smartphone Application to Evaluate Energy Expenditure and Duration of Activities in Free-living Conditions for Overweight and Obese People (eMouve3)</t>
+  </si>
+  <si>
+    <t>Effect of Oral Supplementation With One Form of L-arginine on Vascular Endothelial Function in Healthy Subjects Featuring Risk Factors Related to the Metabolic Syndrome.</t>
   </si>
   <si>
     <t>Effect of Technological Processes on Nutritional Quality of Meat Proteins</t>
@@ -199,12 +205,6 @@
     <t>Preventive Strategies in Colorectal Carcinogenesis Production and Meat Processing</t>
   </si>
   <si>
-    <t>Effect of Oral Supplementation With One Form of L-arginine on Vascular Endothelial Function in Healthy Subjects Featuring Risk Factors Related to the Metabolic Syndrome.</t>
-  </si>
-  <si>
-    <t>A Smartphone Application to Evaluate Energy Expenditure and Duration of Activities in Free-living Conditions for Overweight and Obese People (eMouve3)</t>
-  </si>
-  <si>
     <t>Métabolismes Des caroténoïdes Dans la lumière du Tube Digestif de l'Homme Sain</t>
   </si>
   <si>
@@ -223,12 +223,12 @@
     <t>Fava Bean Protein and Amino Acid Bioavailability in Healthy Volunteers</t>
   </si>
   <si>
+    <t>Effect of Monosodium Glutamate on Gastric Emptying and Postprandial Nitrogen in Healthy Volunteers</t>
+  </si>
+  <si>
     <t>Characterization of the Metabolic Fate of an Oral L-arginine Form in Healthy Subjects Featuring Risk Factors Related to the Metabolic Syndrome.</t>
   </si>
   <si>
-    <t>Effect of Monosodium Glutamate on Gastric Emptying and Postprandial Nitrogen in Healthy Volunteers</t>
-  </si>
-  <si>
     <t>TRANSFACT1</t>
   </si>
   <si>
@@ -238,12 +238,12 @@
     <t>Trans-Insulin</t>
   </si>
   <si>
+    <t>SURPROL-CF-H</t>
+  </si>
+  <si>
     <t>Modelheart</t>
   </si>
   <si>
-    <t>SURPROL-CF-H</t>
-  </si>
-  <si>
     <t>Hemcancer</t>
   </si>
   <si>
@@ -268,16 +268,13 @@
     <t>DIETARY_SUPPLEMENT</t>
   </si>
   <si>
+    <t>OTHER</t>
+  </si>
+  <si>
     <t>DEVICE</t>
   </si>
   <si>
-    <t>OTHER</t>
-  </si>
-  <si>
     <t>BEHAVIORAL</t>
-  </si>
-  <si>
-    <t>DRUG</t>
   </si>
 </sst>
 </file>
@@ -710,7 +707,7 @@
         <v>52</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -793,15 +790,15 @@
         <v>74</v>
       </c>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
@@ -809,16 +806,22 @@
       <c r="F8" t="s">
         <v>43</v>
       </c>
+      <c r="G8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" t="s">
+        <v>75</v>
+      </c>
       <c r="I8" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -827,21 +830,21 @@
         <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H9" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -849,14 +852,8 @@
       <c r="F10" t="s">
         <v>43</v>
       </c>
-      <c r="G10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" t="s">
-        <v>76</v>
-      </c>
       <c r="I10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -876,7 +873,7 @@
         <v>57</v>
       </c>
       <c r="I11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -896,15 +893,15 @@
         <v>58</v>
       </c>
       <c r="I12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -915,16 +912,19 @@
       <c r="G13" t="s">
         <v>59</v>
       </c>
+      <c r="H13" t="s">
+        <v>77</v>
+      </c>
       <c r="I13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>27</v>
@@ -936,15 +936,15 @@
         <v>60</v>
       </c>
       <c r="I14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
         <v>28</v>
@@ -956,7 +956,7 @@
         <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -975,11 +975,8 @@
       <c r="G16" t="s">
         <v>62</v>
       </c>
-      <c r="H16" t="s">
-        <v>77</v>
-      </c>
       <c r="I16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -1002,7 +999,7 @@
         <v>78</v>
       </c>
       <c r="I17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -1025,7 +1022,7 @@
         <v>79</v>
       </c>
       <c r="I18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1045,7 +1042,7 @@
         <v>65</v>
       </c>
       <c r="I19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1091,7 +1088,7 @@
         <v>81</v>
       </c>
       <c r="I21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1119,33 +1116,33 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
         <v>36</v>
       </c>
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
       <c r="I23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
         <v>37</v>
       </c>
-      <c r="G24" t="s">
-        <v>69</v>
-      </c>
       <c r="I24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1158,9 +1155,6 @@
       <c r="C25" t="s">
         <v>38</v>
       </c>
-      <c r="G25" t="s">
-        <v>70</v>
-      </c>
       <c r="I25" t="s">
         <v>83</v>
       </c>
@@ -1174,6 +1168,9 @@
       </c>
       <c r="C26" t="s">
         <v>39</v>
+      </c>
+      <c r="G26" t="s">
+        <v>70</v>
       </c>
       <c r="I26" t="s">
         <v>83</v>

</xml_diff>